<commit_message>
update: csv and xlsx file for the student id to int
</commit_message>
<xml_diff>
--- a/DSTR-Project/docs/100-student-answer.xlsx
+++ b/DSTR-Project/docs/100-student-answer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIGABYTE\Documents\project\DSTR-Project\DSTR-Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726B4BD5-831E-466B-98CB-190ED43C3761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F3231A-1A58-46EC-A978-2EA325F0E408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15540" xr2:uid="{9E45B5A7-7EF5-4C98-A28D-BA5B9A466A4C}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{9E45B5A7-7EF5-4C98-A28D-BA5B9A466A4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -397,18 +397,18 @@
   <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
-        <v>70001</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -420,9 +420,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>70002</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -434,9 +434,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>70003</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -448,9 +448,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>70004</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -462,9 +462,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>70005</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -476,9 +476,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>70006</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -490,9 +490,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>70007</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>0</v>
@@ -504,9 +504,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>70008</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -518,9 +518,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>70009</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
@@ -532,9 +532,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>70010</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
@@ -546,9 +546,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>70011</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>2</v>
@@ -560,9 +560,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>70012</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
@@ -574,9 +574,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>70013</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>0</v>
@@ -588,9 +588,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>70014</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -602,9 +602,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>70015</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>0</v>
@@ -616,9 +616,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>70016</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
@@ -630,9 +630,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>70017</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -644,9 +644,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>70018</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>2</v>
@@ -658,9 +658,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>70019</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>0</v>
@@ -672,9 +672,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>70020</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>3</v>
@@ -686,9 +686,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>70021</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>4</v>
@@ -700,9 +700,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>70022</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>1</v>
@@ -714,9 +714,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>70023</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>2</v>
@@ -728,9 +728,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>70024</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>0</v>
@@ -742,9 +742,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>70025</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>3</v>
@@ -756,9 +756,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>70026</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>4</v>
@@ -770,9 +770,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>70027</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>2</v>
@@ -784,9 +784,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>70028</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>0</v>
@@ -798,9 +798,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>70029</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>3</v>
@@ -812,9 +812,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>70030</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>4</v>
@@ -826,9 +826,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>70031</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>2</v>
@@ -840,9 +840,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>70032</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>1</v>
@@ -854,9 +854,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>70033</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>0</v>
@@ -868,9 +868,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>70034</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>3</v>
@@ -882,9 +882,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>70035</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>4</v>
@@ -896,9 +896,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>70036</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>2</v>
@@ -910,9 +910,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>70037</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>0</v>
@@ -924,9 +924,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>70038</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>3</v>
@@ -938,9 +938,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>70039</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>4</v>
@@ -952,9 +952,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>70040</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>2</v>
@@ -966,9 +966,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>70041</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>0</v>
@@ -980,9 +980,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>70042</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>3</v>
@@ -994,9 +994,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>70043</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>4</v>
@@ -1008,9 +1008,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <v>70044</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>2</v>
@@ -1022,9 +1022,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <v>70045</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>0</v>
@@ -1036,9 +1036,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <v>70046</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>3</v>
@@ -1050,9 +1050,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>70047</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>4</v>
@@ -1064,9 +1064,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <v>70048</v>
+        <v>48</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>2</v>
@@ -1078,9 +1078,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <v>70049</v>
+        <v>49</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>0</v>
@@ -1092,9 +1092,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <v>70050</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>3</v>
@@ -1106,9 +1106,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <v>70051</v>
+        <v>51</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>4</v>
@@ -1120,9 +1120,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <v>70052</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>2</v>
@@ -1134,9 +1134,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <v>70053</v>
+        <v>53</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>0</v>
@@ -1148,9 +1148,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <v>70054</v>
+        <v>54</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>3</v>
@@ -1162,9 +1162,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
-        <v>70055</v>
+        <v>55</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>4</v>
@@ -1176,9 +1176,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <v>70056</v>
+        <v>56</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>2</v>
@@ -1190,9 +1190,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>70057</v>
+        <v>57</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>0</v>
@@ -1204,9 +1204,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <v>70058</v>
+        <v>58</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>3</v>
@@ -1218,9 +1218,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
-        <v>70059</v>
+        <v>59</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>4</v>
@@ -1232,9 +1232,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
-        <v>70060</v>
+        <v>60</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>2</v>
@@ -1246,9 +1246,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
-        <v>70061</v>
+        <v>61</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>0</v>
@@ -1260,9 +1260,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
-        <v>70062</v>
+        <v>62</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>3</v>
@@ -1274,9 +1274,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
-        <v>70063</v>
+        <v>63</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>4</v>
@@ -1288,9 +1288,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
-        <v>70064</v>
+        <v>64</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>2</v>
@@ -1302,9 +1302,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <v>70065</v>
+        <v>65</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>0</v>
@@ -1316,9 +1316,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
-        <v>70066</v>
+        <v>66</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>3</v>
@@ -1330,9 +1330,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <v>70067</v>
+        <v>67</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>4</v>
@@ -1344,9 +1344,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <v>70068</v>
+        <v>68</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>2</v>
@@ -1358,9 +1358,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <v>70069</v>
+        <v>69</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>0</v>
@@ -1372,9 +1372,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>70070</v>
+        <v>70</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>3</v>
@@ -1386,9 +1386,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <v>70071</v>
+        <v>71</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>4</v>
@@ -1400,9 +1400,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
-        <v>70072</v>
+        <v>72</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>2</v>
@@ -1414,9 +1414,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
-        <v>70073</v>
+        <v>73</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>0</v>
@@ -1428,9 +1428,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
-        <v>70074</v>
+        <v>74</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>3</v>
@@ -1442,9 +1442,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <v>70075</v>
+        <v>75</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>4</v>
@@ -1456,9 +1456,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
-        <v>70076</v>
+        <v>76</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>2</v>
@@ -1470,9 +1470,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <v>70077</v>
+        <v>77</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>0</v>
@@ -1484,9 +1484,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <v>70078</v>
+        <v>78</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>3</v>
@@ -1498,9 +1498,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <v>70079</v>
+        <v>79</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>4</v>
@@ -1512,9 +1512,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
-        <v>70080</v>
+        <v>80</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>2</v>
@@ -1526,9 +1526,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
-        <v>70081</v>
+        <v>81</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>0</v>
@@ -1540,9 +1540,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
-        <v>70082</v>
+        <v>82</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>3</v>
@@ -1554,9 +1554,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
-        <v>70083</v>
+        <v>83</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>4</v>
@@ -1568,9 +1568,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
-        <v>70084</v>
+        <v>84</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>2</v>
@@ -1582,9 +1582,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
-        <v>70085</v>
+        <v>85</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>0</v>
@@ -1596,9 +1596,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
-        <v>70086</v>
+        <v>86</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>3</v>
@@ -1610,9 +1610,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
-        <v>70087</v>
+        <v>87</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>4</v>
@@ -1624,9 +1624,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
-        <v>70088</v>
+        <v>88</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>2</v>
@@ -1638,9 +1638,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
-        <v>70089</v>
+        <v>89</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>0</v>
@@ -1652,9 +1652,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
-        <v>70090</v>
+        <v>90</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>3</v>
@@ -1666,9 +1666,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
-        <v>70091</v>
+        <v>91</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>4</v>
@@ -1680,9 +1680,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
-        <v>70092</v>
+        <v>92</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>2</v>
@@ -1694,9 +1694,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
-        <v>70093</v>
+        <v>93</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>0</v>
@@ -1708,9 +1708,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
-        <v>70094</v>
+        <v>94</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>3</v>
@@ -1722,9 +1722,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
-        <v>70095</v>
+        <v>95</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>4</v>
@@ -1736,9 +1736,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
-        <v>70096</v>
+        <v>96</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>2</v>
@@ -1750,9 +1750,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
-        <v>70097</v>
+        <v>97</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>0</v>
@@ -1764,9 +1764,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
-        <v>70098</v>
+        <v>98</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>3</v>
@@ -1778,9 +1778,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
-        <v>70099</v>
+        <v>99</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>4</v>
@@ -1792,9 +1792,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
-        <v>70100</v>
+        <v>100</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>2</v>

</xml_diff>